<commit_message>
Databases week 5 and requirement engineering
</commit_message>
<xml_diff>
--- a/Periode 1.2/Relationele databases/1920-AE&I-IVT1.2-RelDb2-Normaliseren opdracht Sport.xlsx
+++ b/Periode 1.2/Relationele databases/1920-AE&I-IVT1.2-RelDb2-Normaliseren opdracht Sport.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985DE246-E06C-4DA2-B86A-BC3DAC4EB492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF591624-E15D-4F5F-8B20-C585A9914910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>PersoonID</t>
+  </si>
+  <si>
+    <t>Er zijn geen attributen die die afhankelijk zijn van de primareren sleutels</t>
+  </si>
+  <si>
+    <t>Alle tabellen zijn opgesplits</t>
   </si>
 </sst>
 </file>
@@ -224,7 +230,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -512,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBA455B-5E93-40B8-A6C3-D86BD9E6E0C2}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +774,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>0</v>
       </c>
@@ -797,7 +803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>94</v>
       </c>
@@ -825,8 +831,11 @@
       <c r="K19" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>120</v>
       </c>
@@ -854,8 +863,11 @@
       <c r="K20" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>254</v>
       </c>
@@ -884,7 +896,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>312</v>
       </c>
@@ -913,7 +925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>419</v>
       </c>
@@ -942,7 +954,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>426</v>
       </c>
@@ -959,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>476</v>
       </c>
@@ -976,7 +988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>619</v>
       </c>
@@ -993,7 +1005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>828</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28" s="1">
         <v>619</v>
       </c>
@@ -1018,7 +1030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="1">
         <v>828</v>
       </c>
@@ -1079,6 +1091,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF1551BE9D2837459D497D79EE019F1E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d977a3f973d30a279581b2f26bcf14a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81073326-ebee-4c0c-a26a-590ff4adfe90" xmlns:ns3="85fa55d4-3ee8-4bc4-8fbc-63473e847397" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b8fa28db58c16e012f13cc33d56e876c" ns2:_="" ns3:_="">
     <xsd:import namespace="81073326-ebee-4c0c-a26a-590ff4adfe90"/>
@@ -1301,22 +1328,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F503307F-AA9A-40FC-BDB7-B99C38593301}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A13FD54E-8901-4890-876B-C06E392E0BFB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5728709E-809C-44B0-A1A4-A99D40DE5FEB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1333,21 +1362,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A13FD54E-8901-4890-876B-C06E392E0BFB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F503307F-AA9A-40FC-BDB7-B99C38593301}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>